<commit_message>
Modify string to date in xlsx file
</commit_message>
<xml_diff>
--- a/jupyter/data/日本サッカー代表2024.xlsx
+++ b/jupyter/data/日本サッカー代表2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kioto/Desktop/Python講座/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kioto/project/HGSC/python/pyworks/python-sample/jupyter/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43FF1EB-0736-9945-8112-48D898C81C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B6E5AC-9B38-0248-B995-7B4041090DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="8520" windowWidth="28300" windowHeight="17360" xr2:uid="{542797A2-5E95-A540-9A0C-FB7BB9BD77FB}"/>
+    <workbookView xWindow="1940" yWindow="2280" windowWidth="28300" windowHeight="17360" xr2:uid="{542797A2-5E95-A540-9A0C-FB7BB9BD77FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>選手名</t>
   </si>
@@ -65,283 +65,142 @@
     <t>南野 拓実</t>
   </si>
   <si>
-    <t>1995.01.16</t>
-  </si>
-  <si>
     <t>堂安 律</t>
   </si>
   <si>
-    <t>1998.06.16</t>
-  </si>
-  <si>
     <t>鈴木 彩艶</t>
   </si>
   <si>
-    <t>2002.08.21</t>
-  </si>
-  <si>
     <t>板倉 滉</t>
   </si>
   <si>
-    <t>1997.01.27</t>
-  </si>
-  <si>
     <t>遠藤 航</t>
   </si>
   <si>
-    <t>1993.02.09</t>
-  </si>
-  <si>
     <t>町田 浩樹</t>
   </si>
   <si>
-    <t>1997.08.25</t>
-  </si>
-  <si>
     <t>守田 英正</t>
   </si>
   <si>
-    <t>1995.05.10</t>
-  </si>
-  <si>
     <t>上田 綺世</t>
   </si>
   <si>
-    <t>1998.08.28</t>
-  </si>
-  <si>
     <t>久保 建英</t>
   </si>
   <si>
-    <t>2001.06.04</t>
-  </si>
-  <si>
     <t>伊東 純也</t>
   </si>
   <si>
-    <t>1993.03.09</t>
-  </si>
-  <si>
     <t>中村 敬斗</t>
   </si>
   <si>
-    <t>2000.07.28</t>
-  </si>
-  <si>
     <t>前田 大然</t>
   </si>
   <si>
-    <t>1997.10.20</t>
-  </si>
-  <si>
     <t>谷口 彰悟</t>
   </si>
   <si>
-    <t>1991.07.15</t>
-  </si>
-  <si>
     <t>三笘 薫</t>
   </si>
   <si>
-    <t>1997.05.20</t>
-  </si>
-  <si>
     <t>鎌田 大地</t>
   </si>
   <si>
-    <t>1996.08.05</t>
-  </si>
-  <si>
     <t>小川 航基</t>
   </si>
   <si>
-    <t>1997.08.08</t>
-  </si>
-  <si>
     <t>菅原 由勢</t>
   </si>
   <si>
-    <t>2000.06.28</t>
-  </si>
-  <si>
     <t>田中 碧</t>
   </si>
   <si>
-    <t>1998.09.10</t>
-  </si>
-  <si>
     <t>伊藤 洋輝</t>
   </si>
   <si>
-    <t>1999.05.12</t>
-  </si>
-  <si>
     <t>毎熊 晟矢</t>
   </si>
   <si>
-    <t>1997.10.16</t>
-  </si>
-  <si>
     <t>旗手 怜央</t>
   </si>
   <si>
-    <t>1997.11.21</t>
-  </si>
-  <si>
     <t>冨安 健洋</t>
   </si>
   <si>
-    <t>1998.11.05</t>
-  </si>
-  <si>
     <t>浅野 拓磨</t>
   </si>
   <si>
-    <t>1994.11.10</t>
-  </si>
-  <si>
     <t>橋岡 大樹</t>
   </si>
   <si>
-    <t>1999.05.17</t>
-  </si>
-  <si>
     <t>川村 拓夢</t>
   </si>
   <si>
-    <t>1999.08.28</t>
-  </si>
-  <si>
     <t>佐野 海舟</t>
   </si>
   <si>
-    <t>2000.12.30</t>
-  </si>
-  <si>
     <t>細谷 真大</t>
   </si>
   <si>
-    <t>2001.09.07</t>
-  </si>
-  <si>
     <t>中山 雄太</t>
   </si>
   <si>
-    <t>1997.02.16</t>
-  </si>
-  <si>
     <t>相馬 勇紀</t>
   </si>
   <si>
-    <t>1997.02.25</t>
-  </si>
-  <si>
     <t>三浦 颯太</t>
   </si>
   <si>
-    <t>2000.09.07</t>
-  </si>
-  <si>
     <t>伊藤 涼太郎</t>
   </si>
   <si>
-    <t>1998.02.06</t>
-  </si>
-  <si>
     <t>高井 幸大</t>
   </si>
   <si>
-    <t>2004.09.04</t>
-  </si>
-  <si>
     <t>鈴木 唯人</t>
   </si>
   <si>
-    <t>2001.10.25</t>
-  </si>
-  <si>
     <t>奥抜 侃志</t>
   </si>
   <si>
-    <t>1999.08.11</t>
-  </si>
-  <si>
     <t>大橋 祐紀</t>
   </si>
   <si>
-    <t>1996.07.27</t>
-  </si>
-  <si>
     <t>谷 晃生</t>
   </si>
   <si>
-    <t>2000.11.22</t>
-  </si>
-  <si>
     <t>森下 龍矢</t>
   </si>
   <si>
-    <t>1997.04.11</t>
-  </si>
-  <si>
     <t>藤井 陽也</t>
   </si>
   <si>
-    <t>2000.12.26</t>
-  </si>
-  <si>
     <t>瀬古 歩夢</t>
   </si>
   <si>
-    <t>2000.06.07</t>
-  </si>
-  <si>
     <t>渡辺 剛</t>
   </si>
   <si>
-    <t>1997.02.05</t>
-  </si>
-  <si>
     <t>大迫 敬介</t>
   </si>
   <si>
-    <t>1999.07.28</t>
-  </si>
-  <si>
     <t>古橋 亨梧</t>
   </si>
   <si>
-    <t>1995.01.20</t>
-  </si>
-  <si>
     <t>前川 黛也</t>
   </si>
   <si>
-    <t>1994.09.08</t>
-  </si>
-  <si>
     <t>藤田 譲瑠チマ</t>
   </si>
   <si>
-    <t>2002.02.16</t>
-  </si>
-  <si>
     <t>野澤 大志ブランドン</t>
   </si>
   <si>
-    <t>2002.12.25</t>
-  </si>
-  <si>
     <t>長友 佑都</t>
   </si>
   <si>
-    <t>1986.09.12</t>
-  </si>
-  <si>
     <t>望月 ヘンリー海輝</t>
-  </si>
-  <si>
-    <t>2001.09.20</t>
   </si>
 </sst>
 </file>
@@ -401,7 +260,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -409,6 +268,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -748,7 +610,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -785,10 +647,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="B2" s="3">
+        <v>34037</v>
       </c>
       <c r="C2" s="1">
         <v>9</v>
@@ -811,10 +673,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>26</v>
+      </c>
+      <c r="B3" s="3">
+        <v>36292</v>
       </c>
       <c r="C3" s="1">
         <v>6</v>
@@ -837,10 +699,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>38</v>
+      </c>
+      <c r="B4" s="3">
+        <v>35832</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -863,10 +725,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="3">
+        <v>34009</v>
       </c>
       <c r="C5" s="1">
         <v>12</v>
@@ -889,10 +751,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>41</v>
+      </c>
+      <c r="B6" s="3">
+        <v>36383</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -915,10 +777,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="B7" s="3">
+        <v>35282</v>
       </c>
       <c r="C7" s="1">
         <v>7</v>
@@ -941,10 +803,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="B8" s="3">
+        <v>35755</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
@@ -967,10 +829,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="B9" s="3">
+        <v>37046</v>
       </c>
       <c r="C9" s="1">
         <v>10</v>
@@ -993,10 +855,10 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>31</v>
+      </c>
+      <c r="B10" s="3">
+        <v>36297</v>
       </c>
       <c r="C10" s="1">
         <v>4</v>
@@ -1019,10 +881,10 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>49</v>
+      </c>
+      <c r="B11" s="3">
+        <v>34719</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1045,10 +907,10 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>39</v>
+      </c>
+      <c r="B12" s="3">
+        <v>38234</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -1071,10 +933,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>33</v>
+      </c>
+      <c r="B13" s="3">
+        <v>36890</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -1097,10 +959,10 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>34</v>
+      </c>
+      <c r="B14" s="3">
+        <v>37141</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -1123,10 +985,10 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
+      </c>
+      <c r="B15" s="3">
+        <v>36776</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1149,10 +1011,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
+      </c>
+      <c r="B16" s="3">
+        <v>35570</v>
       </c>
       <c r="C16" s="1">
         <v>8</v>
@@ -1175,10 +1037,10 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="B17" s="3">
+        <v>34829</v>
       </c>
       <c r="C17" s="1">
         <v>11</v>
@@ -1201,10 +1063,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
+      </c>
+      <c r="B18" s="3">
+        <v>35650</v>
       </c>
       <c r="C18" s="1">
         <v>7</v>
@@ -1227,10 +1089,10 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="B19" s="3">
+        <v>36035</v>
       </c>
       <c r="C19" s="1">
         <v>11</v>
@@ -1253,10 +1115,10 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
+      </c>
+      <c r="B20" s="3">
+        <v>35531</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -1279,10 +1141,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
+      </c>
+      <c r="B21" s="3">
+        <v>36705</v>
       </c>
       <c r="C21" s="1">
         <v>6</v>
@@ -1305,10 +1167,10 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>46</v>
+      </c>
+      <c r="B22" s="3">
+        <v>36684</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -1331,10 +1193,10 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>32</v>
+      </c>
+      <c r="B23" s="3">
+        <v>36400</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
@@ -1357,10 +1219,10 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
+      </c>
+      <c r="B24" s="3">
+        <v>34648</v>
       </c>
       <c r="C24" s="1">
         <v>4</v>
@@ -1383,10 +1245,10 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>93</v>
+        <v>50</v>
+      </c>
+      <c r="B25" s="3">
+        <v>34585</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -1409,10 +1271,10 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="B26" s="3">
+        <v>35723</v>
       </c>
       <c r="C26" s="1">
         <v>9</v>
@@ -1435,10 +1297,10 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
+      </c>
+      <c r="B27" s="3">
+        <v>35486</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
@@ -1461,10 +1323,10 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>42</v>
+      </c>
+      <c r="B28" s="3">
+        <v>35273</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
@@ -1487,10 +1349,10 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>89</v>
+        <v>48</v>
+      </c>
+      <c r="B29" s="3">
+        <v>36369</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -1513,10 +1375,10 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>43</v>
+      </c>
+      <c r="B30" s="3">
+        <v>36852</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -1539,10 +1401,10 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="B31" s="3">
+        <v>33434</v>
       </c>
       <c r="C31" s="1">
         <v>8</v>
@@ -1565,10 +1427,10 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>35</v>
+      </c>
+      <c r="B32" s="3">
+        <v>35477</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
@@ -1591,10 +1453,10 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="B33" s="3">
+        <v>36735</v>
       </c>
       <c r="C33" s="1">
         <v>9</v>
@@ -1617,10 +1479,10 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B34" s="3">
+        <v>35667</v>
       </c>
       <c r="C34" s="1">
         <v>11</v>
@@ -1643,10 +1505,10 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>99</v>
+        <v>53</v>
+      </c>
+      <c r="B35" s="3">
+        <v>31667</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
@@ -1669,10 +1531,10 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+      <c r="B36" s="3">
+        <v>36048</v>
       </c>
       <c r="C36" s="1">
         <v>6</v>
@@ -1695,10 +1557,10 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>47</v>
+      </c>
+      <c r="B37" s="3">
+        <v>35466</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
@@ -1721,10 +1583,10 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>83</v>
+        <v>45</v>
+      </c>
+      <c r="B38" s="3">
+        <v>36886</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
@@ -1747,10 +1609,10 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>95</v>
+        <v>51</v>
+      </c>
+      <c r="B39" s="3">
+        <v>37303</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
@@ -1773,10 +1635,10 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="B40" s="3">
+        <v>35962</v>
       </c>
       <c r="C40" s="1">
         <v>14</v>
@@ -1801,8 +1663,8 @@
       <c r="A41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>9</v>
+      <c r="B41" s="3">
+        <v>34715</v>
       </c>
       <c r="C41" s="1">
         <v>14</v>
@@ -1825,10 +1687,10 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="B42" s="3">
+        <v>35457</v>
       </c>
       <c r="C42" s="1">
         <v>13</v>
@@ -1851,10 +1713,10 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
+      </c>
+      <c r="B43" s="3">
+        <v>36104</v>
       </c>
       <c r="C43" s="1">
         <v>5</v>
@@ -1877,10 +1739,10 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>101</v>
+        <v>54</v>
+      </c>
+      <c r="B44" s="3">
+        <v>37154</v>
       </c>
       <c r="C44" s="1">
         <v>0</v>
@@ -1903,10 +1765,10 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
+      </c>
+      <c r="B45" s="3">
+        <v>35719</v>
       </c>
       <c r="C45" s="1">
         <v>5</v>
@@ -1929,10 +1791,10 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>97</v>
+        <v>52</v>
+      </c>
+      <c r="B46" s="3">
+        <v>37615</v>
       </c>
       <c r="C46" s="1">
         <v>0</v>
@@ -1955,10 +1817,10 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="B47" s="3">
+        <v>37489</v>
       </c>
       <c r="C47" s="1">
         <v>13</v>
@@ -1981,10 +1843,10 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>73</v>
+        <v>40</v>
+      </c>
+      <c r="B48" s="3">
+        <v>37189</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>

</xml_diff>